<commit_message>
fix deleting active tahun-pelajaran issue
- system should not delete an active tahun-pelajaran data
</commit_message>
<xml_diff>
--- a/public/template/Data Pembayaran Komite Semester Genap.xlsx
+++ b/public/template/Data Pembayaran Komite Semester Genap.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="27 jmy 6" sheetId="1" r:id="rId4"/>
-    <sheet name="12 MIA 2" sheetId="2" r:id="rId5"/>
-    <sheet name="04 gbk 2" sheetId="3" r:id="rId6"/>
+    <sheet name="24 wao 6" sheetId="1" r:id="rId4"/>
+    <sheet name="45 iie 1" sheetId="2" r:id="rId5"/>
+    <sheet name="49 sbj 7" sheetId="3" r:id="rId6"/>
+    <sheet name="12 MIA 2" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -17,18 +18,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>DAFTAR PEMBAYARAN ADMINISTRASI KOMITE</t>
   </si>
   <si>
-    <t>TAHUN AJARAN 20329</t>
+    <t>TAHUN AJARAN 2022/2023</t>
   </si>
   <si>
     <t>SEMESTER GENAP (II)</t>
   </si>
   <si>
-    <t>KELAS 27 jmy 6</t>
+    <t>KELAS 24 wao 6</t>
   </si>
   <si>
     <t>NO</t>
@@ -64,37 +65,85 @@
     <t>JUNI</t>
   </si>
   <si>
-    <t>Silvia Nurdiyanti</t>
-  </si>
-  <si>
-    <t>Rp. 0</t>
+    <t>Farah Prastuti</t>
+  </si>
+  <si>
+    <t>Rp. 420.000</t>
   </si>
   <si>
     <t>Belum Lunas</t>
   </si>
   <si>
-    <t>Siska Genta Hasanah M.Ak</t>
-  </si>
-  <si>
-    <t>Rp. 420.000</t>
-  </si>
-  <si>
-    <t>Hudi Gloria</t>
+    <t>Almira Padmasari S.E.I</t>
+  </si>
+  <si>
+    <t>Wahyu Dongoran</t>
+  </si>
+  <si>
+    <t>Citra Yolanda</t>
+  </si>
+  <si>
+    <t>KELAS 45 iie 1</t>
+  </si>
+  <si>
+    <t>Diana Padmasari</t>
+  </si>
+  <si>
+    <t>Lunas</t>
+  </si>
+  <si>
+    <t>Saiful Sihotang</t>
+  </si>
+  <si>
+    <t>Cakrabirawa Narpati S.Ked</t>
+  </si>
+  <si>
+    <t>Kamila Aryani</t>
+  </si>
+  <si>
+    <t>Zulaikha Zalindra Yuniar</t>
+  </si>
+  <si>
+    <t>KELAS 49 sbj 7</t>
+  </si>
+  <si>
+    <t>Koko Wahyudin</t>
+  </si>
+  <si>
+    <t>Tasdik Lazuardi</t>
+  </si>
+  <si>
+    <t>Kenari Darsirah Situmorang M.Kom.</t>
+  </si>
+  <si>
+    <t>Danang Wahyudin</t>
+  </si>
+  <si>
+    <t>Ibun Dongoran</t>
+  </si>
+  <si>
+    <t>Sarah Agustina</t>
   </si>
   <si>
     <t>KELAS 12 MIA 2</t>
   </si>
   <si>
-    <t>Yosef Mustofa</t>
-  </si>
-  <si>
-    <t>Lunas</t>
-  </si>
-  <si>
-    <t>KELAS 04 gbk 2</t>
-  </si>
-  <si>
-    <t>sadsads fe</t>
+    <t>Himawan Maheswara</t>
+  </si>
+  <si>
+    <t>Dagel Tasnim Wasita</t>
+  </si>
+  <si>
+    <t>Harjasa Mangunsong</t>
+  </si>
+  <si>
+    <t>Nalar Lazuardi</t>
+  </si>
+  <si>
+    <t>Maida Unjani Sudiati</t>
+  </si>
+  <si>
+    <t>Wd</t>
   </si>
 </sst>
 </file>
@@ -606,7 +655,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,7 +778,7 @@
       <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -764,7 +813,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>17</v>
@@ -794,44 +843,64 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:17" customHeight="1" ht="21.9">
       <c r="A12" s="1"/>
@@ -1266,7 +1335,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1389,11 +1458,11 @@
       <c r="B8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="21" t="s">
         <v>23</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>17</v>
@@ -1417,53 +1486,133 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:17" customHeight="1" ht="21.9">
       <c r="A13" s="1"/>
@@ -1885,8 +2034,8 @@
   </sheetPr>
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1950,7 +2099,7 @@
     </row>
     <row r="5" spans="1:17" customHeight="1" ht="15.6">
       <c r="A5" s="17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" s="17"/>
     </row>
@@ -2007,10 +2156,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>17</v>
@@ -2037,65 +2186,885 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:17" customHeight="1" ht="21.9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A16" s="1"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A17" s="1"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A18" s="1"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A21" s="1"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A22" s="1"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A23" s="1"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A24" s="1"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A26" s="1"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A27" s="1"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A28" s="1"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A29" s="1"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A30" s="1"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A31" s="1"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A33" s="1"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A34" s="1"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A35" s="1"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A36" s="1"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A37" s="1"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A38" s="1"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A39" s="1"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A40" s="1"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A41" s="1"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A42" s="1"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+    </row>
+    <row r="43" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A43" s="1"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A44" s="2"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+    </row>
+    <row r="45" spans="1:17" customHeight="1" ht="21.9"/>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.23622047244094" right="0.23622047244094" top="0.74803149606299" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="70" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="true" style="0"/>
+    <col min="2" max="2" width="29.5546875" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.5546875" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13.77734375" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13.6640625" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.5546875" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.5546875" customWidth="true" style="0"/>
+    <col min="8" max="8" width="13" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12.5546875" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.5546875" customWidth="true" style="0"/>
+    <col min="15" max="15" width="8.88671875" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11.33203125" customWidth="true" style="0"/>
+    <col min="17" max="17" width="12.88671875" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" customHeight="1" ht="18">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:17" customHeight="1" ht="18">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:17" customHeight="1" ht="18">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="5" spans="1:17" customHeight="1" ht="15.6">
+      <c r="A5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" customHeight="1" ht="21.9">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:17" customHeight="1" ht="21.9">
       <c r="A14" s="1"/>

</xml_diff>